<commit_message>
some import and export stuff
</commit_message>
<xml_diff>
--- a/app/static/import-examples.xlsx
+++ b/app/static/import-examples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="19200" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="19200" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Import-examples" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>The following examples are valid, gray columns will not be imported or taken into account</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>NAME</t>
+  </si>
+  <si>
+    <t>Columns that must be present: name, club</t>
+  </si>
+  <si>
+    <t>optional columns: id (must have a header)</t>
+  </si>
+  <si>
+    <t>duplicate id's will be replaced with another id</t>
   </si>
 </sst>
 </file>
@@ -678,7 +687,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -689,12 +698,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1016,11 +1026,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M34"/>
+  <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1041,6 +1049,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
@@ -1307,10 +1323,10 @@
       <c r="D28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1321,10 +1337,10 @@
       <c r="D29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="15">
         <v>1</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1333,10 +1349,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="8"/>
-      <c r="E30" s="12">
+      <c r="E30" s="15">
         <v>2</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1347,10 +1363,10 @@
       <c r="D31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="12">
-        <v>3</v>
-      </c>
-      <c r="F31" s="13" t="s">
+      <c r="E31" s="11">
+        <v>2</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1361,24 +1377,29 @@
       <c r="D32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="15">
         <v>4</v>
       </c>
-      <c r="F32" s="13"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="5"/>
       <c r="D33" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="16">
         <v>5</v>
       </c>
-      <c r="F33" s="15"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- rename event to category properly, i thought i did this ages ago... - fix dd pres order for intl and se - import members column as well when importing participants from excel
</commit_message>
<xml_diff>
--- a/app/static/import-examples.xlsx
+++ b/app/static/import-examples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00svbeon\Desktop\RopeScore\app\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hemarbete\.babun\cygwin\home\00svbeon\git\RopeScore\app\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="19200" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="19200" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Import-examples" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
   <si>
     <t>The following examples are valid, gray columns will not be imported or taken into account</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Variation 3:</t>
   </si>
   <si>
-    <t>(can also consist of headers (first row) can be with any capitalization as long as they don't start or end with a space)</t>
-  </si>
-  <si>
     <t>Example 3:</t>
   </si>
   <si>
@@ -114,10 +111,61 @@
     <t>Columns that must be present: name, club</t>
   </si>
   <si>
-    <t>optional columns: id (must have a header)</t>
-  </si>
-  <si>
     <t>duplicate id's will be replaced with another id</t>
+  </si>
+  <si>
+    <t>optional columns: id (must have a header), members</t>
+  </si>
+  <si>
+    <t>(can also consist of headers (first row) can be with any capitalization</t>
+  </si>
+  <si>
+    <t>Example 5:</t>
+  </si>
+  <si>
+    <t>Team BEST</t>
+  </si>
+  <si>
+    <t>Team better</t>
+  </si>
+  <si>
+    <t>Team rock</t>
+  </si>
+  <si>
+    <t>Team teaming</t>
+  </si>
+  <si>
+    <t>Name, Nam</t>
+  </si>
+  <si>
+    <t>Nom, Nim</t>
+  </si>
+  <si>
+    <t>Num, Nem</t>
+  </si>
+  <si>
+    <t>Nym</t>
+  </si>
+  <si>
+    <t>(can be without headers if the first column is names, the second is clubs and the third one is members)</t>
+  </si>
+  <si>
+    <t>members</t>
+  </si>
+  <si>
+    <t>Louvenia, Cinda  </t>
+  </si>
+  <si>
+    <t>Daryl, Marquitta  </t>
+  </si>
+  <si>
+    <t>Tillie, Charolett</t>
+  </si>
+  <si>
+    <t>Roman, Angel</t>
+  </si>
+  <si>
+    <t>Karine, Al, Cher</t>
   </si>
 </sst>
 </file>
@@ -687,7 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -698,13 +746,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,9 +1078,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M35"/>
+  <dimension ref="B3:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1044,20 +1098,20 @@
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1068,13 +1122,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1090,319 +1144,395 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K19" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="2" t="s">
+      <c r="L19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="F14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="I14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="L14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="I21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="L21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="15">
-        <v>1</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="15">
-        <v>2</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="13">
+        <v>1</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="13">
+        <v>2</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E38" s="10">
         <v>2</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F38" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="13">
+        <v>4</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="14">
+        <v>5</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="15">
-        <v>4</v>
-      </c>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="16">
-        <v>5</v>
-      </c>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>32</v>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>